<commit_message>
inversed some efficiency calcs. and cleaning
</commit_message>
<xml_diff>
--- a/documentation/model_simulation.xlsx
+++ b/documentation/model_simulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://aperc-my.sharepoint.com/personal/finbar_maunsell_aperc_or_jp/Documents/Documents/Github/transport_model_9th_edition/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\APERC\transport_model_9th_edition\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2526" documentId="8_{8502E8ED-7478-4F46-8E14-35AF7EA2E2DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{620EF0BF-FF7C-42EE-99A3-55AB46FFA600}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB368548-A1A9-4E1A-A08E-B562712AC4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-15" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FC33B140-7E9F-4908-90CB-09BAA5341BE8}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="122">
   <si>
     <t>vehicle type</t>
   </si>
@@ -437,6 +437,9 @@
   </si>
   <si>
     <t>Activity worth of extra stocks remaining</t>
+  </si>
+  <si>
+    <t>total energy use (travel km / efficiency)</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -598,7 +601,6 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -4195,8 +4197,8 @@
   </sheetPr>
   <dimension ref="A1:BQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AB56" sqref="AB56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -4598,7 +4600,7 @@
       <c r="N9" t="s">
         <v>109</v>
       </c>
-      <c r="O9" s="17" t="s">
+      <c r="O9" s="16" t="s">
         <v>111</v>
       </c>
     </row>
@@ -4652,7 +4654,7 @@
         <f>(M10)*J2*G10</f>
         <v>104.5</v>
       </c>
-      <c r="O10" s="17">
+      <c r="O10" s="16">
         <f>SUM(N$10:N$15)</f>
         <v>126.1</v>
       </c>
@@ -4710,7 +4712,7 @@
         <f t="shared" ref="N11:N15" si="8">(M11)*J3*G11</f>
         <v>9.0000000000000018</v>
       </c>
-      <c r="O11" s="17">
+      <c r="O11" s="16">
         <f t="shared" ref="O11:O15" si="9">SUM(N$10:N$15)</f>
         <v>126.1</v>
       </c>
@@ -4765,7 +4767,7 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O12" s="17">
+      <c r="O12" s="16">
         <f t="shared" si="9"/>
         <v>126.1</v>
       </c>
@@ -4820,7 +4822,7 @@
         <f t="shared" si="8"/>
         <v>3.6000000000000005</v>
       </c>
-      <c r="O13" s="17">
+      <c r="O13" s="16">
         <f t="shared" si="9"/>
         <v>126.1</v>
       </c>
@@ -4875,7 +4877,7 @@
         <f t="shared" si="8"/>
         <v>4.5</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="16">
         <f t="shared" si="9"/>
         <v>126.1</v>
       </c>
@@ -4930,7 +4932,7 @@
         <f t="shared" si="8"/>
         <v>4.5</v>
       </c>
-      <c r="O15" s="17">
+      <c r="O15" s="16">
         <f t="shared" si="9"/>
         <v>126.1</v>
       </c>
@@ -4975,7 +4977,7 @@
       <c r="M17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="15" t="s">
+      <c r="N17" t="s">
         <v>112</v>
       </c>
       <c r="O17" s="11" t="s">
@@ -4999,7 +5001,7 @@
       <c r="U17" t="s">
         <v>42</v>
       </c>
-      <c r="V17" s="16" t="s">
+      <c r="V17" s="15" t="s">
         <v>22</v>
       </c>
       <c r="W17" s="11" t="s">
@@ -5018,7 +5020,7 @@
         <v>107</v>
       </c>
       <c r="AB17" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:69" x14ac:dyDescent="0.4">
@@ -5050,42 +5052,42 @@
         <v>-4.3499999999999996</v>
       </c>
       <c r="I18" s="11">
-        <f>IF(O10-G18-H18&lt;0, O10-G18-H18,0)</f>
+        <f t="shared" ref="I18:I23" si="10">IF(O10-G18-H18&lt;0, O10-G18-H18,0)</f>
         <v>0</v>
       </c>
       <c r="J18" s="11">
-        <f>IF(O10-G18-H18&gt;0, O10-G18-H18,0)</f>
+        <f t="shared" ref="J18:J23" si="11">IF(O10-G18-H18&gt;0, O10-G18-H18,0)</f>
         <v>101.44999999999999</v>
       </c>
       <c r="K18">
-        <f>J18/O10</f>
+        <f t="shared" ref="K18:K23" si="12">J18/O10</f>
         <v>0.80452022204599516</v>
       </c>
       <c r="L18">
-        <f>K18*N10</f>
+        <f t="shared" ref="L18:L23" si="13">K18*N10</f>
         <v>84.072363203806489</v>
       </c>
       <c r="M18" s="1">
         <v>0.142355008787346</v>
       </c>
-      <c r="N18" s="15">
+      <c r="N18">
         <f>I18*M18</f>
         <v>0</v>
       </c>
       <c r="O18" s="11">
-        <f>N10+N18-L18</f>
+        <f t="shared" ref="O18:O23" si="14">N10+N18-L18</f>
         <v>20.427636796193511</v>
       </c>
       <c r="P18">
-        <f>O18/G10</f>
+        <f t="shared" ref="P18:P23" si="15">O18/G10</f>
         <v>13.618424530795673</v>
       </c>
       <c r="Q18">
-        <f>N18/G10</f>
+        <f t="shared" ref="Q18:Q23" si="16">N18/G10</f>
         <v>0</v>
       </c>
       <c r="R18">
-        <f>L18/G10</f>
+        <f t="shared" ref="R18:R23" si="17">L18/G10</f>
         <v>56.048242135870993</v>
       </c>
       <c r="S18" s="2">
@@ -5093,11 +5095,11 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="T18">
-        <f>P18/S18</f>
+        <f t="shared" ref="T18:T23" si="18">P18/S18</f>
         <v>20.427636796193507</v>
       </c>
       <c r="U18">
-        <f>Q18/S18</f>
+        <f t="shared" ref="U18:U23" si="19">Q18/S18</f>
         <v>0</v>
       </c>
       <c r="V18">
@@ -5105,27 +5107,27 @@
         <v>84.072363203806475</v>
       </c>
       <c r="W18" s="11">
-        <f>T18-U18</f>
+        <f t="shared" ref="W18:W23" si="20">T18-U18</f>
         <v>20.427636796193507</v>
       </c>
       <c r="X18" s="13">
-        <f>H2</f>
+        <f t="shared" ref="X18:X23" si="21">H2</f>
         <v>1.2</v>
       </c>
       <c r="Y18" s="1">
         <v>1.0833333333333299</v>
       </c>
       <c r="Z18">
-        <f>Y18*H2</f>
+        <f t="shared" ref="Z18:Z23" si="22">Y18*H2</f>
         <v>1.2999999999999958</v>
       </c>
       <c r="AA18" s="11">
-        <f>IF(T18=0,Z18,(IF(U18&lt;0,H2,((U18*Z18)+(W18*H2))/(T18))))</f>
+        <f t="shared" ref="AA18:AA23" si="23">IF(T18=0,Z18,(IF(U18&lt;0,H2,((U18*Z18)+(W18*H2))/(T18))))</f>
         <v>1.2</v>
       </c>
       <c r="AB18">
-        <f>AA18*P18</f>
-        <v>16.342109436954807</v>
+        <f>P18/AA18</f>
+        <v>11.348687108996394</v>
       </c>
       <c r="BQ18" t="s">
         <v>24</v>
@@ -5152,61 +5154,61 @@
         <v>-0.15</v>
       </c>
       <c r="G19">
-        <f t="shared" ref="G19:G23" si="10">SUM(F$2:F$7)</f>
+        <f t="shared" ref="G19:G23" si="24">SUM(F$2:F$7)</f>
         <v>29</v>
       </c>
       <c r="H19">
-        <f t="shared" ref="H19:H23" si="11">(F19*G19)</f>
+        <f t="shared" ref="H19:H23" si="25">(F19*G19)</f>
         <v>-4.3499999999999996</v>
       </c>
       <c r="I19" s="11">
-        <f>IF(O11-G19-H19&lt;0, O11-G19-H19,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J19" s="11">
-        <f>IF(O11-G19-H19&gt;0, O11-G19-H19,0)</f>
+        <f t="shared" si="11"/>
         <v>101.44999999999999</v>
       </c>
       <c r="K19">
-        <f>J19/O11</f>
+        <f t="shared" si="12"/>
         <v>0.80452022204599516</v>
       </c>
       <c r="L19">
-        <f>K19*N11</f>
+        <f t="shared" si="13"/>
         <v>7.2406819984139581</v>
       </c>
       <c r="M19" s="1">
         <v>0.284710017574692</v>
       </c>
-      <c r="N19" s="15">
-        <f t="shared" ref="N19:N23" si="12">I19*M19</f>
+      <c r="N19">
+        <f t="shared" ref="N19:N23" si="26">I19*M19</f>
         <v>0</v>
       </c>
       <c r="O19" s="11">
-        <f>N11+N19-L19</f>
+        <f t="shared" si="14"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="P19">
-        <f>O19/G11</f>
+        <f t="shared" si="15"/>
         <v>1.172878667724029</v>
       </c>
       <c r="Q19">
-        <f>N19/G11</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R19">
-        <f>L19/G11</f>
+        <f t="shared" si="17"/>
         <v>4.8271213322759721</v>
       </c>
       <c r="S19" s="2">
         <v>0.66666666666666674</v>
       </c>
       <c r="T19">
-        <f>P19/S19</f>
+        <f t="shared" si="18"/>
         <v>1.7593180015860435</v>
       </c>
       <c r="U19">
-        <f>Q19/S19</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V19">
@@ -5214,27 +5216,27 @@
         <v>7.2406819984139572</v>
       </c>
       <c r="W19" s="11">
-        <f>T19-U19</f>
+        <f t="shared" si="20"/>
         <v>1.7593180015860435</v>
       </c>
       <c r="X19" s="13">
-        <f>H3</f>
+        <f t="shared" si="21"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="Y19" s="1">
         <v>1.0909090909090908</v>
       </c>
       <c r="Z19">
-        <f>Y19*H3</f>
+        <f t="shared" si="22"/>
         <v>1.2</v>
       </c>
       <c r="AA19" s="11">
-        <f>IF(T19=0,Z19,(IF(U19&lt;0,H3,((U19*Z19)+(W19*H3))/(T19))))</f>
+        <f t="shared" si="23"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AB19">
-        <f>AA19*P19</f>
-        <v>1.2901665344964321</v>
+        <f t="shared" ref="AB19:AB23" si="27">P19/AA19</f>
+        <v>1.0662533342945717</v>
       </c>
     </row>
     <row r="20" spans="1:69" x14ac:dyDescent="0.4">
@@ -5266,42 +5268,42 @@
         <v>-4.3499999999999996</v>
       </c>
       <c r="I20" s="11">
-        <f>IF(O12-G20-H20&lt;0, O12-G20-H20,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="J20" s="11">
-        <f>IF(O12-G20-H20&gt;0, O12-G20-H20,0)</f>
+        <f t="shared" si="11"/>
         <v>101.44999999999999</v>
       </c>
       <c r="K20">
-        <f>J20/O12</f>
+        <f t="shared" si="12"/>
         <v>0.80452022204599516</v>
       </c>
       <c r="L20">
-        <f>K20*N12</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="M20" s="1">
         <v>5.4481546572934969E-2</v>
       </c>
-      <c r="N20" s="15">
-        <f t="shared" si="12"/>
+      <c r="N20">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O20" s="11">
-        <f>N12+N20-L20</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="P20">
-        <f>O20/G12</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q20">
-        <f>N20/G12</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R20">
-        <f>L20/G12</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="S20" s="2">
@@ -5309,38 +5311,38 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="T20">
-        <f>P20/S20</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="U20">
-        <f>Q20/S20</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V20">
-        <f t="shared" ref="V20:V23" si="13">R20/S20</f>
+        <f t="shared" ref="V20:V23" si="28">R20/S20</f>
         <v>0</v>
       </c>
       <c r="W20" s="11">
-        <f>T20-U20</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="X20" s="13">
-        <f>H4</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="Y20" s="1">
         <v>1.05</v>
       </c>
       <c r="Z20">
-        <f>Y20*H4</f>
+        <f t="shared" si="22"/>
         <v>2.1</v>
       </c>
       <c r="AA20" s="11">
-        <f>IF(T20=0,Z20,(IF(U20&lt;0,H4,((U20*Z20)+(W20*H4))/(T20))))</f>
+        <f t="shared" si="23"/>
         <v>2.1</v>
       </c>
       <c r="AB20">
-        <f>AA20*P20</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
     </row>
@@ -5361,93 +5363,93 @@
         <v>98</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" ref="F21:F22" si="14">F20</f>
+        <f t="shared" ref="F21:F22" si="29">F20</f>
         <v>-0.15</v>
       </c>
       <c r="G21">
+        <f t="shared" si="24"/>
+        <v>29</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="25"/>
+        <v>-4.3499999999999996</v>
+      </c>
+      <c r="I21" s="11">
         <f t="shared" si="10"/>
-        <v>29</v>
-      </c>
-      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21" s="11">
         <f t="shared" si="11"/>
-        <v>-4.3499999999999996</v>
-      </c>
-      <c r="I21" s="11">
-        <f>IF(O13-G21-H21&lt;0, O13-G21-H21,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J21" s="11">
-        <f>IF(O13-G21-H21&gt;0, O13-G21-H21,0)</f>
         <v>101.44999999999999</v>
       </c>
       <c r="K21">
-        <f>J21/O13</f>
+        <f t="shared" si="12"/>
         <v>0.80452022204599516</v>
       </c>
       <c r="L21">
-        <f>K21*N13</f>
+        <f t="shared" si="13"/>
         <v>2.8962727993655828</v>
       </c>
       <c r="M21" s="1">
         <v>0.34270650263620378</v>
       </c>
-      <c r="N21" s="15">
-        <f t="shared" si="12"/>
+      <c r="N21">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O21" s="11">
-        <f>N13+N21-L21</f>
+        <f t="shared" si="14"/>
         <v>0.70372720063441774</v>
       </c>
       <c r="P21">
-        <f>O21/G13</f>
+        <f t="shared" si="15"/>
         <v>0.58643933386201486</v>
       </c>
       <c r="Q21">
-        <f>N21/G13</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R21">
-        <f>L21/G13</f>
+        <f t="shared" si="17"/>
         <v>2.4135606661379856</v>
       </c>
       <c r="S21" s="2">
         <v>0.66666666666666674</v>
       </c>
       <c r="T21">
-        <f>P21/S21</f>
+        <f t="shared" si="18"/>
         <v>0.87965900079302217</v>
       </c>
       <c r="U21">
-        <f>Q21/S21</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V21">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>3.6203409992069782</v>
       </c>
       <c r="W21" s="11">
-        <f>T21-U21</f>
+        <f t="shared" si="20"/>
         <v>0.87965900079302217</v>
       </c>
       <c r="X21" s="13">
-        <f>H5</f>
+        <f t="shared" si="21"/>
         <v>2</v>
       </c>
       <c r="Y21" s="1">
         <v>1.05</v>
       </c>
       <c r="Z21">
-        <f>Y21*H5</f>
+        <f t="shared" si="22"/>
         <v>2.1</v>
       </c>
       <c r="AA21" s="11">
-        <f>IF(T21=0,Z21,(IF(U21&lt;0,H5,((U21*Z21)+(W21*H5))/(T21))))</f>
+        <f t="shared" si="23"/>
         <v>2</v>
       </c>
       <c r="AB21">
-        <f>AA21*P21</f>
-        <v>1.1728786677240297</v>
+        <f t="shared" si="27"/>
+        <v>0.29321966693100743</v>
       </c>
     </row>
     <row r="22" spans="1:69" x14ac:dyDescent="0.4">
@@ -5467,92 +5469,92 @@
         <v>7</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="29"/>
         <v>-0.15</v>
       </c>
       <c r="G22">
+        <f t="shared" si="24"/>
+        <v>29</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="25"/>
+        <v>-4.3499999999999996</v>
+      </c>
+      <c r="I22" s="11">
         <f t="shared" si="10"/>
-        <v>29</v>
-      </c>
-      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="J22" s="11">
         <f t="shared" si="11"/>
-        <v>-4.3499999999999996</v>
-      </c>
-      <c r="I22" s="11">
-        <f>IF(O14-G22-H22&lt;0, O14-G22-H22,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="11">
-        <f>IF(O14-G22-H22&gt;0, O14-G22-H22,0)</f>
         <v>101.44999999999999</v>
       </c>
       <c r="K22">
-        <f>J22/O14</f>
+        <f t="shared" si="12"/>
         <v>0.80452022204599516</v>
       </c>
       <c r="L22">
-        <f>K22*N14</f>
+        <f t="shared" si="13"/>
         <v>3.6203409992069782</v>
       </c>
       <c r="M22" s="1">
         <v>8.7873462214411238E-2</v>
       </c>
-      <c r="N22" s="15">
-        <f t="shared" si="12"/>
+      <c r="N22">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O22" s="11">
-        <f>N14+N22-L22</f>
+        <f t="shared" si="14"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="P22">
-        <f>O22/G14</f>
+        <f t="shared" si="15"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="Q22">
-        <f>N22/G14</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R22">
-        <f>L22/G14</f>
+        <f t="shared" si="17"/>
         <v>3.6203409992069782</v>
       </c>
       <c r="S22" s="2">
         <v>0.5</v>
       </c>
       <c r="T22">
-        <f>P22/S22</f>
+        <f t="shared" si="18"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="U22">
-        <f>Q22/S22</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V22">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>7.2406819984139563</v>
       </c>
       <c r="W22" s="11">
-        <f>T22-U22</f>
+        <f t="shared" si="20"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="X22" s="13">
-        <f>H6</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="Y22" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="Z22">
-        <f>Y22*H6</f>
+        <f t="shared" si="22"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA22" s="11">
-        <f>IF(T22=0,Z22,(IF(U22&lt;0,H6,((U22*Z22)+(W22*H6))/(T22))))</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="AB22">
-        <f>AA22*P22</f>
+        <f t="shared" si="27"/>
         <v>0.87965900079302184</v>
       </c>
     </row>
@@ -5577,88 +5579,88 @@
         <v>-0.15</v>
       </c>
       <c r="G23">
+        <f t="shared" si="24"/>
+        <v>29</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="25"/>
+        <v>-4.3499999999999996</v>
+      </c>
+      <c r="I23" s="11">
         <f t="shared" si="10"/>
-        <v>29</v>
-      </c>
-      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="J23" s="11">
         <f t="shared" si="11"/>
-        <v>-4.3499999999999996</v>
-      </c>
-      <c r="I23" s="11">
-        <f>IF(O15-G23-H23&lt;0, O15-G23-H23,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J23" s="11">
-        <f>IF(O15-G23-H23&gt;0, O15-G23-H23,0)</f>
         <v>101.44999999999999</v>
       </c>
       <c r="K23">
-        <f>J23/O15</f>
+        <f t="shared" si="12"/>
         <v>0.80452022204599516</v>
       </c>
       <c r="L23">
-        <f>K23*N15</f>
+        <f t="shared" si="13"/>
         <v>3.6203409992069782</v>
       </c>
       <c r="M23" s="1">
         <v>8.7873462214411238E-2</v>
       </c>
-      <c r="N23" s="15">
-        <f t="shared" si="12"/>
+      <c r="N23">
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O23" s="11">
-        <f>N15+N23-L23</f>
+        <f t="shared" si="14"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="P23">
-        <f>O23/G15</f>
+        <f t="shared" si="15"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="Q23">
-        <f>N23/G15</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="R23">
-        <f>L23/G15</f>
+        <f t="shared" si="17"/>
         <v>3.6203409992069782</v>
       </c>
       <c r="S23" s="2">
         <v>0.5</v>
       </c>
       <c r="T23">
-        <f>P23/S23</f>
+        <f t="shared" si="18"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="U23">
-        <f>Q23/S23</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="V23">
-        <f t="shared" si="13"/>
+        <f t="shared" si="28"/>
         <v>7.2406819984139563</v>
       </c>
       <c r="W23" s="11">
-        <f>T23-U23</f>
+        <f t="shared" si="20"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="X23" s="13">
-        <f>H7</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="Y23" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="Z23">
-        <f>Y23*H7</f>
+        <f t="shared" si="22"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA23" s="11">
-        <f>IF(T23=0,Z23,(IF(U23&lt;0,H7,((U23*Z23)+(W23*H7))/(T23))))</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="AB23">
-        <f>AA23*P23</f>
+        <f t="shared" si="27"/>
         <v>0.87965900079302184</v>
       </c>
     </row>
@@ -5712,7 +5714,7 @@
       </c>
       <c r="H26" s="7">
         <f>G26*AB18</f>
-        <v>16.342109436954807</v>
+        <v>11.348687108996394</v>
       </c>
       <c r="T26" s="6"/>
       <c r="BN26" t="s">
@@ -5743,7 +5745,7 @@
       </c>
       <c r="H27" s="7">
         <f>G27*AB19</f>
-        <v>1.1611498810467891</v>
+        <v>0.95962800086511457</v>
       </c>
       <c r="T27" s="6"/>
     </row>
@@ -5771,7 +5773,7 @@
       </c>
       <c r="H28" s="7">
         <f>G28*AB19</f>
-        <v>0.12901665344964322</v>
+        <v>0.10662533342945718</v>
       </c>
       <c r="T28" s="6"/>
     </row>
@@ -5883,7 +5885,7 @@
       </c>
       <c r="H32" s="7">
         <f>G32*AB21</f>
-        <v>0.52779540047581341</v>
+        <v>0.13194885011895335</v>
       </c>
       <c r="T32" s="6"/>
     </row>
@@ -5911,7 +5913,7 @@
       </c>
       <c r="H33" s="7">
         <f>G33*AB21</f>
-        <v>0.46915146708961192</v>
+        <v>0.11728786677240298</v>
       </c>
       <c r="T33" s="6"/>
     </row>
@@ -5939,7 +5941,7 @@
       </c>
       <c r="H34" s="7">
         <f>G34*AB21</f>
-        <v>5.864393338620149E-2</v>
+        <v>1.4660983346550372E-2</v>
       </c>
       <c r="T34" s="6"/>
     </row>
@@ -6088,23 +6090,23 @@
         <v>7</v>
       </c>
       <c r="F40" s="7">
-        <f>O18</f>
+        <f t="shared" ref="F40:F45" si="30">O18</f>
         <v>20.427636796193511</v>
       </c>
       <c r="G40" s="7">
-        <f>T18</f>
+        <f t="shared" ref="G40:G45" si="31">T18</f>
         <v>20.427636796193507</v>
       </c>
       <c r="H40" s="7">
-        <f>AA18</f>
+        <f t="shared" ref="H40:I45" si="32">AA18</f>
         <v>1.2</v>
       </c>
       <c r="I40" s="7">
-        <f>AB18</f>
-        <v>16.342109436954807</v>
+        <f t="shared" si="32"/>
+        <v>11.348687108996394</v>
       </c>
       <c r="J40" s="10">
-        <f>IFERROR(L40/G40,S18)</f>
+        <f t="shared" ref="J40:J45" si="33">IFERROR(L40/G40,S18)</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="K40">
@@ -6112,7 +6114,7 @@
         <v>1.5</v>
       </c>
       <c r="L40">
-        <f>P18</f>
+        <f t="shared" ref="L40:L45" si="34">P18</f>
         <v>13.618424530795673</v>
       </c>
       <c r="M40" s="11">
@@ -6141,39 +6143,39 @@
         <v>8</v>
       </c>
       <c r="F41" s="7">
-        <f>O19</f>
+        <f t="shared" si="30"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="G41" s="7">
-        <f>T19</f>
+        <f t="shared" si="31"/>
         <v>1.7593180015860435</v>
       </c>
       <c r="H41" s="7">
-        <f>AA19</f>
+        <f t="shared" si="32"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="I41" s="7">
-        <f>AB19</f>
-        <v>1.2901665344964321</v>
+        <f t="shared" si="32"/>
+        <v>1.0662533342945717</v>
       </c>
       <c r="J41" s="10">
-        <f>IFERROR(L41/G41,S19)</f>
+        <f t="shared" si="33"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K41">
-        <f t="shared" ref="K41:K45" si="15">G11</f>
+        <f t="shared" ref="K41:K45" si="35">G11</f>
         <v>1.5</v>
       </c>
       <c r="L41">
-        <f>P19</f>
+        <f t="shared" si="34"/>
         <v>1.172878667724029</v>
       </c>
       <c r="M41" s="11">
-        <f t="shared" ref="M41:M45" si="16">V19</f>
+        <f t="shared" ref="M41:M45" si="36">V19</f>
         <v>7.2406819984139572</v>
       </c>
       <c r="N41">
-        <f t="shared" ref="N41:N45" si="17">I11</f>
+        <f t="shared" ref="N41:N45" si="37">I11</f>
         <v>0.1</v>
       </c>
     </row>
@@ -6194,39 +6196,39 @@
         <v>98</v>
       </c>
       <c r="F42" s="7">
-        <f>O20</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="G42" s="7">
-        <f>T20</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H42" s="7">
-        <f>AA20</f>
+        <f t="shared" si="32"/>
         <v>2.1</v>
       </c>
       <c r="I42" s="7">
-        <f>AB20</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="J42" s="10">
-        <f>IFERROR(L42/G42,S20)</f>
+        <f t="shared" si="33"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K42">
-        <f t="shared" si="15"/>
+        <f t="shared" si="35"/>
         <v>1.2</v>
       </c>
       <c r="L42">
-        <f>P20</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="M42" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="N42">
-        <f t="shared" si="17"/>
+        <f t="shared" si="37"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6247,39 +6249,39 @@
         <v>98</v>
       </c>
       <c r="F43" s="7">
-        <f>O21</f>
+        <f t="shared" si="30"/>
         <v>0.70372720063441774</v>
       </c>
       <c r="G43" s="7">
-        <f>T21</f>
+        <f t="shared" si="31"/>
         <v>0.87965900079302217</v>
       </c>
       <c r="H43" s="7">
-        <f>AA21</f>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="I43" s="7">
-        <f>AB21</f>
-        <v>1.1728786677240297</v>
+        <f t="shared" si="32"/>
+        <v>0.29321966693100743</v>
       </c>
       <c r="J43" s="10">
-        <f>IFERROR(L43/G43,S21)</f>
+        <f t="shared" si="33"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K43">
-        <f t="shared" si="15"/>
+        <f t="shared" si="35"/>
         <v>1.2</v>
       </c>
       <c r="L43">
-        <f>P21</f>
+        <f t="shared" si="34"/>
         <v>0.58643933386201486</v>
       </c>
       <c r="M43" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>3.6203409992069782</v>
       </c>
       <c r="N43">
-        <f t="shared" si="17"/>
+        <f t="shared" si="37"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6300,39 +6302,39 @@
         <v>7</v>
       </c>
       <c r="F44" s="7">
-        <f>O22</f>
+        <f t="shared" si="30"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="G44" s="7">
-        <f>T22</f>
+        <f t="shared" si="31"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="H44" s="7">
-        <f>AA22</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="I44" s="7">
-        <f>AB22</f>
+        <f t="shared" si="32"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="J44" s="10">
-        <f>IFERROR(L44/G44,S22)</f>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="K44">
-        <f t="shared" si="15"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="L44">
-        <f>P22</f>
+        <f t="shared" si="34"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="M44" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>7.2406819984139563</v>
       </c>
       <c r="N44">
-        <f t="shared" si="17"/>
+        <f t="shared" si="37"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6353,39 +6355,39 @@
         <v>8</v>
       </c>
       <c r="F45" s="7">
-        <f>O23</f>
+        <f t="shared" si="30"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="G45" s="7">
-        <f>T23</f>
+        <f t="shared" si="31"/>
         <v>1.7593180015860437</v>
       </c>
       <c r="H45" s="7">
-        <f>AA23</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="I45" s="7">
-        <f>AB23</f>
+        <f t="shared" si="32"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="J45" s="10">
-        <f>IFERROR(L45/G45,S23)</f>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="K45">
-        <f t="shared" si="15"/>
+        <f t="shared" si="35"/>
         <v>1</v>
       </c>
       <c r="L45">
-        <f>P23</f>
+        <f t="shared" si="34"/>
         <v>0.87965900079302184</v>
       </c>
       <c r="M45" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="36"/>
         <v>7.2406819984139563</v>
       </c>
       <c r="N45">
-        <f t="shared" si="17"/>
+        <f t="shared" si="37"/>
         <v>0.1</v>
       </c>
     </row>
@@ -6435,7 +6437,7 @@
       <c r="N47" t="s">
         <v>109</v>
       </c>
-      <c r="O47" s="17" t="s">
+      <c r="O47" s="16" t="s">
         <v>111</v>
       </c>
     </row>
@@ -6489,7 +6491,7 @@
         <f>(M48)*J40*G48</f>
         <v>102.45703204401269</v>
       </c>
-      <c r="O48" s="17">
+      <c r="O48" s="16">
         <f>SUM(N$48:N$53)</f>
         <v>123.63475350000002</v>
       </c>
@@ -6517,38 +6519,38 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <f t="shared" ref="G49:G53" si="18">K41*F49</f>
+        <f t="shared" ref="G49:G53" si="38">K41*F49</f>
         <v>1.5</v>
       </c>
       <c r="H49" s="1">
         <v>1.0001</v>
       </c>
       <c r="I49">
-        <f t="shared" ref="I49:I53" si="19">N41*H49</f>
+        <f t="shared" ref="I49:I53" si="39">N41*H49</f>
         <v>0.10001</v>
       </c>
       <c r="J49">
-        <f t="shared" ref="J49:J53" si="20">G41*I49</f>
+        <f t="shared" ref="J49:J53" si="40">G41*I49</f>
         <v>0.1759493933386202</v>
       </c>
       <c r="K49">
-        <f t="shared" ref="K49:K53" si="21">-J49+M41</f>
+        <f t="shared" ref="K49:K53" si="41">-J49+M41</f>
         <v>7.0647326050753367</v>
       </c>
       <c r="L49">
-        <f t="shared" ref="L49:L53" si="22">(K49)*J41*G49</f>
+        <f t="shared" ref="L49:L53" si="42">(K49)*J41*G49</f>
         <v>7.0647326050753376</v>
       </c>
       <c r="M49">
-        <f t="shared" ref="M49:M53" si="23">G41+K49</f>
+        <f t="shared" ref="M49:M53" si="43">G41+K49</f>
         <v>8.8240506066613804</v>
       </c>
       <c r="N49">
-        <f t="shared" ref="N49:N53" si="24">(M49)*J41*G49</f>
+        <f t="shared" ref="N49:N53" si="44">(M49)*J41*G49</f>
         <v>8.8240506066613804</v>
       </c>
-      <c r="O49" s="17">
-        <f t="shared" ref="O49:O53" si="25">SUM(N$48:N$53)</f>
+      <c r="O49" s="16">
+        <f t="shared" ref="O49:O53" si="45">SUM(N$48:N$53)</f>
         <v>123.63475350000002</v>
       </c>
     </row>
@@ -6572,38 +6574,38 @@
         <v>1</v>
       </c>
       <c r="G50">
-        <f t="shared" si="18"/>
+        <f t="shared" si="38"/>
         <v>1.2</v>
       </c>
       <c r="H50" s="1">
         <v>1.0001</v>
       </c>
       <c r="I50">
-        <f t="shared" si="19"/>
+        <f t="shared" si="39"/>
         <v>0.10001</v>
       </c>
       <c r="J50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="K50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="L50">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="M50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="N50">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="O50" s="17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="O50" s="16">
+        <f t="shared" si="45"/>
         <v>123.63475350000002</v>
       </c>
     </row>
@@ -6627,38 +6629,38 @@
         <v>1</v>
       </c>
       <c r="G51">
-        <f t="shared" si="18"/>
+        <f t="shared" si="38"/>
         <v>1.2</v>
       </c>
       <c r="H51" s="1">
         <v>1.0001</v>
       </c>
       <c r="I51">
-        <f t="shared" si="19"/>
+        <f t="shared" si="39"/>
         <v>0.10001</v>
       </c>
       <c r="J51">
-        <f t="shared" si="20"/>
+        <f t="shared" si="40"/>
         <v>8.7974696669310154E-2</v>
       </c>
       <c r="K51">
-        <f t="shared" si="21"/>
+        <f t="shared" si="41"/>
         <v>3.5323663025376679</v>
       </c>
       <c r="L51">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>2.8258930420301343</v>
       </c>
       <c r="M51">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>4.4120253033306902</v>
       </c>
       <c r="N51">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>3.5296202426645524</v>
       </c>
-      <c r="O51" s="17">
-        <f t="shared" si="25"/>
+      <c r="O51" s="16">
+        <f t="shared" si="45"/>
         <v>123.63475350000002</v>
       </c>
     </row>
@@ -6682,38 +6684,38 @@
         <v>1</v>
       </c>
       <c r="G52">
-        <f t="shared" si="18"/>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="H52" s="1">
         <v>1.0001</v>
       </c>
       <c r="I52">
-        <f t="shared" si="19"/>
+        <f t="shared" si="39"/>
         <v>0.10001</v>
       </c>
       <c r="J52">
-        <f t="shared" si="20"/>
+        <f t="shared" si="40"/>
         <v>0.17594939333862022</v>
       </c>
       <c r="K52">
-        <f t="shared" si="21"/>
+        <f t="shared" si="41"/>
         <v>7.0647326050753358</v>
       </c>
       <c r="L52">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>3.5323663025376679</v>
       </c>
       <c r="M52">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>8.8240506066613804</v>
       </c>
       <c r="N52">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>4.4120253033306902</v>
       </c>
-      <c r="O52" s="17">
-        <f t="shared" si="25"/>
+      <c r="O52" s="16">
+        <f t="shared" si="45"/>
         <v>123.63475350000002</v>
       </c>
     </row>
@@ -6737,38 +6739,38 @@
         <v>1</v>
       </c>
       <c r="G53">
-        <f t="shared" si="18"/>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="H53" s="1">
         <v>1.0001</v>
       </c>
       <c r="I53">
-        <f t="shared" si="19"/>
+        <f t="shared" si="39"/>
         <v>0.10001</v>
       </c>
       <c r="J53">
-        <f t="shared" si="20"/>
+        <f t="shared" si="40"/>
         <v>0.17594939333862022</v>
       </c>
       <c r="K53">
-        <f t="shared" si="21"/>
+        <f t="shared" si="41"/>
         <v>7.0647326050753358</v>
       </c>
       <c r="L53">
-        <f t="shared" si="22"/>
+        <f t="shared" si="42"/>
         <v>3.5323663025376679</v>
       </c>
       <c r="M53">
-        <f t="shared" si="23"/>
+        <f t="shared" si="43"/>
         <v>8.8240506066613804</v>
       </c>
       <c r="N53">
-        <f t="shared" si="24"/>
+        <f t="shared" si="44"/>
         <v>4.4120253033306902</v>
       </c>
-      <c r="O53" s="17">
-        <f t="shared" si="25"/>
+      <c r="O53" s="16">
+        <f t="shared" si="45"/>
         <v>123.63475350000002</v>
       </c>
     </row>
@@ -6812,7 +6814,7 @@
       <c r="M55" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="N55" s="15" t="s">
+      <c r="N55" t="s">
         <v>112</v>
       </c>
       <c r="O55" s="11" t="s">
@@ -6836,7 +6838,7 @@
       <c r="U55" t="s">
         <v>42</v>
       </c>
-      <c r="V55" s="16" t="s">
+      <c r="V55" s="15" t="s">
         <v>22</v>
       </c>
       <c r="W55" s="11" t="s">
@@ -6883,46 +6885,46 @@
         <v>24.65000000000002</v>
       </c>
       <c r="H56">
-        <f t="shared" ref="H56:H61" si="26">(F56*G56)</f>
+        <f t="shared" ref="H56:H61" si="46">(F56*G56)</f>
         <v>-3.6975000000000029</v>
       </c>
       <c r="I56" s="11">
-        <f>IF(O48-G56-H56&lt;0, O48-G56-H56,0)</f>
+        <f t="shared" ref="I56:I61" si="47">IF(O48-G56-H56&lt;0, O48-G56-H56,0)</f>
         <v>0</v>
       </c>
       <c r="J56" s="11">
-        <f>IF(O48-G56-H56&gt;0, O48-G56-H56,0)</f>
+        <f t="shared" ref="J56:J61" si="48">IF(O48-G56-H56&gt;0, O48-G56-H56,0)</f>
         <v>102.6822535</v>
       </c>
       <c r="K56">
-        <f>J56/O48</f>
+        <f t="shared" ref="K56:K61" si="49">J56/O48</f>
         <v>0.83052904295231189</v>
       </c>
       <c r="L56">
-        <f>K56*N48</f>
+        <f t="shared" ref="L56:L61" si="50">K56*N48</f>
         <v>85.093540767248214</v>
       </c>
       <c r="M56" s="1">
         <v>0.142355008787346</v>
       </c>
-      <c r="N56" s="15">
+      <c r="N56">
         <f>I56*M56</f>
         <v>0</v>
       </c>
       <c r="O56" s="11">
-        <f>N48+N56-L56</f>
+        <f t="shared" ref="O56:O61" si="51">N48+N56-L56</f>
         <v>17.363491276764478</v>
       </c>
       <c r="P56">
-        <f>O56/G48</f>
+        <f t="shared" ref="P56:P61" si="52">O56/G48</f>
         <v>11.575660851176318</v>
       </c>
       <c r="Q56">
-        <f>N56/G48</f>
+        <f t="shared" ref="Q56:Q61" si="53">N56/G48</f>
         <v>0</v>
       </c>
       <c r="R56">
-        <f>L56/G48</f>
+        <f t="shared" ref="R56:R61" si="54">L56/G48</f>
         <v>56.729027178165474</v>
       </c>
       <c r="S56" s="2">
@@ -6930,11 +6932,11 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="T56">
-        <f>P56/S56</f>
+        <f t="shared" ref="T56:T61" si="55">P56/S56</f>
         <v>17.363491276764474</v>
       </c>
       <c r="U56">
-        <f>Q56/S56</f>
+        <f t="shared" ref="U56:U61" si="56">Q56/S56</f>
         <v>0</v>
       </c>
       <c r="V56">
@@ -6942,27 +6944,27 @@
         <v>85.0935407672482</v>
       </c>
       <c r="W56" s="11">
-        <f>T56-U56</f>
+        <f t="shared" ref="W56:W61" si="57">T56-U56</f>
         <v>17.363491276764474</v>
       </c>
       <c r="X56" s="13">
-        <f>H40</f>
+        <f t="shared" ref="X56:X61" si="58">H40</f>
         <v>1.2</v>
       </c>
       <c r="Y56" s="1">
         <v>1.0833333333333299</v>
       </c>
       <c r="Z56">
-        <f>Y56*H40</f>
+        <f t="shared" ref="Z56:Z61" si="59">Y56*H40</f>
         <v>1.2999999999999958</v>
       </c>
       <c r="AA56" s="11">
-        <f>IF(T56=0,Z56,(IF(U56&lt;0,H40,((U56*Z56)+(W56*H40))/(T56))))</f>
+        <f t="shared" ref="AA56:AA61" si="60">IF(T56=0,Z56,(IF(U56&lt;0,H40,((U56*Z56)+(W56*H40))/(T56))))</f>
         <v>1.2</v>
       </c>
       <c r="AB56">
-        <f>AA56*P56</f>
-        <v>13.89079302141158</v>
+        <f>P56/AA56</f>
+        <v>9.6463840426469325</v>
       </c>
     </row>
     <row r="57" spans="1:66" x14ac:dyDescent="0.4">
@@ -6986,61 +6988,61 @@
         <v>-0.15</v>
       </c>
       <c r="G57">
-        <f t="shared" ref="G57:G61" si="27">SUM(F$40:F$45)</f>
+        <f t="shared" ref="G57:G61" si="61">SUM(F$40:F$45)</f>
         <v>24.65000000000002</v>
       </c>
       <c r="H57">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-3.6975000000000029</v>
       </c>
       <c r="I57" s="11">
-        <f>IF(O49-G57-H57&lt;0, O49-G57-H57,0)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J57" s="11">
-        <f>IF(O49-G57-H57&gt;0, O49-G57-H57,0)</f>
+        <f t="shared" si="48"/>
         <v>102.6822535</v>
       </c>
       <c r="K57">
-        <f>J57/O49</f>
+        <f t="shared" si="49"/>
         <v>0.83052904295231189</v>
       </c>
       <c r="L57">
-        <f>K57*N49</f>
+        <f t="shared" si="50"/>
         <v>7.3286303053132436</v>
       </c>
       <c r="M57" s="1">
         <v>0.284710017574692</v>
       </c>
-      <c r="N57" s="15">
-        <f t="shared" ref="N57:N61" si="28">I57*M57</f>
+      <c r="N57">
+        <f t="shared" ref="N57:N61" si="62">I57*M57</f>
         <v>0</v>
       </c>
       <c r="O57" s="11">
-        <f>N49+N57-L57</f>
+        <f t="shared" si="51"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="P57">
-        <f>O57/G49</f>
+        <f t="shared" si="52"/>
         <v>0.99694686756542461</v>
       </c>
       <c r="Q57">
-        <f>N57/G49</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R57">
-        <f>L57/G49</f>
+        <f t="shared" si="54"/>
         <v>4.8857535368754954</v>
       </c>
       <c r="S57" s="2">
         <v>0.66666666666666674</v>
       </c>
       <c r="T57">
-        <f>P57/S57</f>
+        <f t="shared" si="55"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="U57">
-        <f>Q57/S57</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V57">
@@ -7048,27 +7050,27 @@
         <v>7.3286303053132427</v>
       </c>
       <c r="W57" s="11">
-        <f>T57-U57</f>
+        <f t="shared" si="57"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="X57" s="13">
-        <f>H41</f>
+        <f t="shared" si="58"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="Y57" s="1">
         <v>1.0909090909090908</v>
       </c>
       <c r="Z57">
-        <f>Y57*H41</f>
+        <f t="shared" si="59"/>
         <v>1.2</v>
       </c>
       <c r="AA57" s="11">
-        <f>IF(T57=0,Z57,(IF(U57&lt;0,H41,((U57*Z57)+(W57*H41))/(T57))))</f>
+        <f t="shared" si="60"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AB57">
-        <f>AA57*P57</f>
-        <v>1.0966415543219672</v>
+        <f t="shared" ref="AB57:AB61" si="63">P57/AA57</f>
+        <v>0.9063153341503859</v>
       </c>
     </row>
     <row r="58" spans="1:66" x14ac:dyDescent="0.4">
@@ -7092,50 +7094,50 @@
         <v>-0.15</v>
       </c>
       <c r="G58">
-        <f t="shared" si="27"/>
+        <f t="shared" si="61"/>
         <v>24.65000000000002</v>
       </c>
       <c r="H58">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-3.6975000000000029</v>
       </c>
       <c r="I58" s="11">
-        <f>IF(O50-G58-H58&lt;0, O50-G58-H58,0)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J58" s="11">
-        <f>IF(O50-G58-H58&gt;0, O50-G58-H58,0)</f>
+        <f t="shared" si="48"/>
         <v>102.6822535</v>
       </c>
       <c r="K58">
-        <f>J58/O50</f>
+        <f t="shared" si="49"/>
         <v>0.83052904295231189</v>
       </c>
       <c r="L58">
-        <f>K58*N50</f>
+        <f t="shared" si="50"/>
         <v>0</v>
       </c>
       <c r="M58" s="1">
         <v>5.4481546572934969E-2</v>
       </c>
-      <c r="N58" s="15">
-        <f t="shared" si="28"/>
+      <c r="N58">
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O58" s="11">
-        <f>N50+N58-L58</f>
+        <f t="shared" si="51"/>
         <v>0</v>
       </c>
       <c r="P58">
-        <f>O58/G50</f>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Q58">
-        <f>N58/G50</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R58">
-        <f>L58/G50</f>
+        <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="S58" s="2">
@@ -7143,38 +7145,38 @@
         <v>0.66666666666666674</v>
       </c>
       <c r="T58">
-        <f>P58/S58</f>
+        <f t="shared" si="55"/>
         <v>0</v>
       </c>
       <c r="U58">
-        <f>Q58/S58</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V58">
-        <f t="shared" ref="V58:V61" si="29">R58/S58</f>
+        <f t="shared" ref="V58:V61" si="64">R58/S58</f>
         <v>0</v>
       </c>
       <c r="W58" s="11">
-        <f>T58-U58</f>
+        <f t="shared" si="57"/>
         <v>0</v>
       </c>
       <c r="X58" s="13">
-        <f>H42</f>
+        <f t="shared" si="58"/>
         <v>2.1</v>
       </c>
       <c r="Y58" s="1">
         <v>1.05</v>
       </c>
       <c r="Z58">
-        <f>Y58*H42</f>
+        <f t="shared" si="59"/>
         <v>2.2050000000000001</v>
       </c>
       <c r="AA58" s="11">
-        <f>IF(T58=0,Z58,(IF(U58&lt;0,H42,((U58*Z58)+(W58*H42))/(T58))))</f>
+        <f t="shared" si="60"/>
         <v>2.2050000000000001</v>
       </c>
       <c r="AB58">
-        <f>AA58*P58</f>
+        <f t="shared" si="63"/>
         <v>0</v>
       </c>
     </row>
@@ -7195,93 +7197,93 @@
         <v>98</v>
       </c>
       <c r="F59" s="1">
-        <f t="shared" ref="F59:F60" si="30">F58</f>
+        <f t="shared" ref="F59:F60" si="65">F58</f>
         <v>-0.15</v>
       </c>
       <c r="G59">
-        <f t="shared" si="27"/>
+        <f t="shared" si="61"/>
         <v>24.65000000000002</v>
       </c>
       <c r="H59">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-3.6975000000000029</v>
       </c>
       <c r="I59" s="11">
-        <f>IF(O51-G59-H59&lt;0, O51-G59-H59,0)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J59" s="11">
-        <f>IF(O51-G59-H59&gt;0, O51-G59-H59,0)</f>
+        <f t="shared" si="48"/>
         <v>102.6822535</v>
       </c>
       <c r="K59">
-        <f>J59/O51</f>
+        <f t="shared" si="49"/>
         <v>0.83052904295231189</v>
       </c>
       <c r="L59">
-        <f>K59*N51</f>
+        <f t="shared" si="50"/>
         <v>2.9314521221252976</v>
       </c>
       <c r="M59" s="1">
         <v>0.34270650263620378</v>
       </c>
-      <c r="N59" s="15">
-        <f t="shared" si="28"/>
+      <c r="N59">
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O59" s="11">
-        <f>N51+N59-L59</f>
+        <f t="shared" si="51"/>
         <v>0.59816812053925483</v>
       </c>
       <c r="P59">
-        <f>O59/G51</f>
+        <f t="shared" si="52"/>
         <v>0.49847343378271236</v>
       </c>
       <c r="Q59">
-        <f>N59/G51</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R59">
-        <f>L59/G51</f>
+        <f t="shared" si="54"/>
         <v>2.4428767684377481</v>
       </c>
       <c r="S59" s="2">
         <v>0.66666666666666674</v>
       </c>
       <c r="T59">
-        <f>P59/S59</f>
+        <f t="shared" si="55"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="U59">
-        <f>Q59/S59</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V59">
-        <f t="shared" si="29"/>
+        <f t="shared" si="64"/>
         <v>3.6643151526566218</v>
       </c>
       <c r="W59" s="11">
-        <f>T59-U59</f>
+        <f t="shared" si="57"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="X59" s="13">
-        <f>H43</f>
+        <f t="shared" si="58"/>
         <v>2</v>
       </c>
       <c r="Y59" s="1">
         <v>1.05</v>
       </c>
       <c r="Z59">
-        <f>Y59*H43</f>
+        <f t="shared" si="59"/>
         <v>2.1</v>
       </c>
       <c r="AA59" s="11">
-        <f>IF(T59=0,Z59,(IF(U59&lt;0,H43,((U59*Z59)+(W59*H43))/(T59))))</f>
+        <f t="shared" si="60"/>
         <v>2</v>
       </c>
       <c r="AB59">
-        <f>AA59*P59</f>
-        <v>0.99694686756542472</v>
+        <f t="shared" si="63"/>
+        <v>0.24923671689135618</v>
       </c>
     </row>
     <row r="60" spans="1:66" x14ac:dyDescent="0.4">
@@ -7301,92 +7303,92 @@
         <v>7</v>
       </c>
       <c r="F60" s="1">
-        <f t="shared" si="30"/>
+        <f t="shared" si="65"/>
         <v>-0.15</v>
       </c>
       <c r="G60">
-        <f t="shared" si="27"/>
+        <f t="shared" si="61"/>
         <v>24.65000000000002</v>
       </c>
       <c r="H60">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-3.6975000000000029</v>
       </c>
       <c r="I60" s="11">
-        <f>IF(O52-G60-H60&lt;0, O52-G60-H60,0)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J60" s="11">
-        <f>IF(O52-G60-H60&gt;0, O52-G60-H60,0)</f>
+        <f t="shared" si="48"/>
         <v>102.6822535</v>
       </c>
       <c r="K60">
-        <f>J60/O52</f>
+        <f t="shared" si="49"/>
         <v>0.83052904295231189</v>
       </c>
       <c r="L60">
-        <f>K60*N52</f>
+        <f t="shared" si="50"/>
         <v>3.6643151526566218</v>
       </c>
       <c r="M60" s="1">
         <v>8.7873462214411238E-2</v>
       </c>
-      <c r="N60" s="15">
-        <f t="shared" si="28"/>
+      <c r="N60">
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O60" s="11">
-        <f>N52+N60-L60</f>
+        <f t="shared" si="51"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="P60">
-        <f>O60/G52</f>
+        <f t="shared" si="52"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="Q60">
-        <f>N60/G52</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R60">
-        <f>L60/G52</f>
+        <f t="shared" si="54"/>
         <v>3.6643151526566218</v>
       </c>
       <c r="S60" s="2">
         <v>0.5</v>
       </c>
       <c r="T60">
-        <f>P60/S60</f>
+        <f t="shared" si="55"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="U60">
-        <f>Q60/S60</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V60">
-        <f t="shared" si="29"/>
+        <f t="shared" si="64"/>
         <v>7.3286303053132436</v>
       </c>
       <c r="W60" s="11">
-        <f>T60-U60</f>
+        <f t="shared" si="57"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="X60" s="13">
-        <f>H44</f>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="Y60" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="Z60">
-        <f>Y60*H44</f>
+        <f t="shared" si="59"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA60" s="11">
-        <f>IF(T60=0,Z60,(IF(U60&lt;0,H44,((U60*Z60)+(W60*H44))/(T60))))</f>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="AB60">
-        <f>AA60*P60</f>
+        <f t="shared" si="63"/>
         <v>0.74771015067406843</v>
       </c>
     </row>
@@ -7411,88 +7413,88 @@
         <v>-0.15</v>
       </c>
       <c r="G61">
-        <f t="shared" si="27"/>
+        <f t="shared" si="61"/>
         <v>24.65000000000002</v>
       </c>
       <c r="H61">
-        <f t="shared" si="26"/>
+        <f t="shared" si="46"/>
         <v>-3.6975000000000029</v>
       </c>
       <c r="I61" s="11">
-        <f>IF(O53-G61-H61&lt;0, O53-G61-H61,0)</f>
+        <f t="shared" si="47"/>
         <v>0</v>
       </c>
       <c r="J61" s="11">
-        <f>IF(O53-G61-H61&gt;0, O53-G61-H61,0)</f>
+        <f t="shared" si="48"/>
         <v>102.6822535</v>
       </c>
       <c r="K61">
-        <f>J61/O53</f>
+        <f t="shared" si="49"/>
         <v>0.83052904295231189</v>
       </c>
       <c r="L61">
-        <f>K61*N53</f>
+        <f t="shared" si="50"/>
         <v>3.6643151526566218</v>
       </c>
       <c r="M61" s="1">
         <v>8.7873462214411238E-2</v>
       </c>
-      <c r="N61" s="15">
-        <f t="shared" si="28"/>
+      <c r="N61">
+        <f t="shared" si="62"/>
         <v>0</v>
       </c>
       <c r="O61" s="11">
-        <f>N53+N61-L61</f>
+        <f t="shared" si="51"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="P61">
-        <f>O61/G53</f>
+        <f t="shared" si="52"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="Q61">
-        <f>N61/G53</f>
+        <f t="shared" si="53"/>
         <v>0</v>
       </c>
       <c r="R61">
-        <f>L61/G53</f>
+        <f t="shared" si="54"/>
         <v>3.6643151526566218</v>
       </c>
       <c r="S61" s="2">
         <v>0.5</v>
       </c>
       <c r="T61">
-        <f>P61/S61</f>
+        <f t="shared" si="55"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="U61">
-        <f>Q61/S61</f>
+        <f t="shared" si="56"/>
         <v>0</v>
       </c>
       <c r="V61">
-        <f t="shared" si="29"/>
+        <f t="shared" si="64"/>
         <v>7.3286303053132436</v>
       </c>
       <c r="W61" s="11">
-        <f>T61-U61</f>
+        <f t="shared" si="57"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="X61" s="13">
-        <f>H45</f>
+        <f t="shared" si="58"/>
         <v>1</v>
       </c>
       <c r="Y61" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="Z61">
-        <f>Y61*H45</f>
+        <f t="shared" si="59"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="AA61" s="11">
-        <f>IF(T61=0,Z61,(IF(U61&lt;0,H45,((U61*Z61)+(W61*H45))/(T61))))</f>
+        <f t="shared" si="60"/>
         <v>1</v>
       </c>
       <c r="AB61">
-        <f>AA61*P61</f>
+        <f t="shared" si="63"/>
         <v>0.74771015067406843</v>
       </c>
     </row>
@@ -7546,7 +7548,7 @@
       </c>
       <c r="H64" s="7">
         <f>G64*AB56</f>
-        <v>13.89079302141158</v>
+        <v>9.6463840426469325</v>
       </c>
       <c r="T64" s="6"/>
       <c r="BN64" t="s">
@@ -7577,7 +7579,7 @@
       </c>
       <c r="H65" s="7">
         <f>G65*AB57</f>
-        <v>0.98697739888977054</v>
+        <v>0.8156838007353473</v>
       </c>
       <c r="T65" s="6"/>
     </row>
@@ -7605,7 +7607,7 @@
       </c>
       <c r="H66" s="7">
         <f>G66*AB57</f>
-        <v>0.10966415543219672</v>
+        <v>9.0631533415038601E-2</v>
       </c>
       <c r="T66" s="6"/>
     </row>
@@ -7717,7 +7719,7 @@
       </c>
       <c r="H70" s="7">
         <f>G70*AB59</f>
-        <v>0.44862609040444112</v>
+        <v>0.11215652260111028</v>
       </c>
       <c r="T70" s="6"/>
     </row>
@@ -7745,7 +7747,7 @@
       </c>
       <c r="H71" s="7">
         <f>G71*AB59</f>
-        <v>0.39877874702616989</v>
+        <v>9.9694686756542472E-2</v>
       </c>
       <c r="T71" s="6"/>
     </row>
@@ -7773,7 +7775,7 @@
       </c>
       <c r="H72" s="7">
         <f>G72*AB59</f>
-        <v>4.9847343378271236E-2</v>
+        <v>1.2461835844567809E-2</v>
       </c>
       <c r="T72" s="6"/>
     </row>
@@ -7922,23 +7924,23 @@
         <v>7</v>
       </c>
       <c r="F78" s="7">
-        <f>O56</f>
+        <f t="shared" ref="F78:F83" si="66">O56</f>
         <v>17.363491276764478</v>
       </c>
       <c r="G78" s="7">
-        <f>T56</f>
+        <f t="shared" ref="G78:G83" si="67">T56</f>
         <v>17.363491276764474</v>
       </c>
       <c r="H78" s="7">
-        <f>AA56</f>
+        <f t="shared" ref="H78:I83" si="68">AA56</f>
         <v>1.2</v>
       </c>
       <c r="I78" s="7">
-        <f>AB56</f>
-        <v>13.89079302141158</v>
+        <f t="shared" si="68"/>
+        <v>9.6463840426469325</v>
       </c>
       <c r="J78" s="10">
-        <f>IFERROR(L78/G78,S56)</f>
+        <f t="shared" ref="J78:J83" si="69">IFERROR(L78/G78,S56)</f>
         <v>0.66666666666666674</v>
       </c>
       <c r="K78">
@@ -7946,7 +7948,7 @@
         <v>1.5</v>
       </c>
       <c r="L78">
-        <f>P56</f>
+        <f t="shared" ref="L78:L83" si="70">P56</f>
         <v>11.575660851176318</v>
       </c>
       <c r="M78" s="11">
@@ -7975,39 +7977,39 @@
         <v>8</v>
       </c>
       <c r="F79" s="7">
-        <f>O57</f>
+        <f t="shared" si="66"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="G79" s="7">
-        <f>T57</f>
+        <f t="shared" si="67"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="H79" s="7">
-        <f>AA57</f>
+        <f t="shared" si="68"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="I79" s="7">
-        <f>AB57</f>
-        <v>1.0966415543219672</v>
+        <f t="shared" si="68"/>
+        <v>0.9063153341503859</v>
       </c>
       <c r="J79" s="10">
-        <f>IFERROR(L79/G79,S57)</f>
+        <f t="shared" si="69"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K79">
-        <f t="shared" ref="K79:K83" si="31">G49</f>
+        <f t="shared" ref="K79:K83" si="71">G49</f>
         <v>1.5</v>
       </c>
       <c r="L79">
-        <f>P57</f>
+        <f t="shared" si="70"/>
         <v>0.99694686756542461</v>
       </c>
       <c r="M79" s="11">
-        <f t="shared" ref="M79:M83" si="32">V57</f>
+        <f t="shared" ref="M79:M83" si="72">V57</f>
         <v>7.3286303053132427</v>
       </c>
       <c r="N79">
-        <f t="shared" ref="N79:N83" si="33">I49</f>
+        <f t="shared" ref="N79:N83" si="73">I49</f>
         <v>0.10001</v>
       </c>
     </row>
@@ -8028,39 +8030,39 @@
         <v>98</v>
       </c>
       <c r="F80" s="7">
-        <f>O58</f>
+        <f t="shared" si="66"/>
         <v>0</v>
       </c>
       <c r="G80" s="7">
-        <f>T58</f>
+        <f t="shared" si="67"/>
         <v>0</v>
       </c>
       <c r="H80" s="7">
-        <f>AA58</f>
+        <f t="shared" si="68"/>
         <v>2.2050000000000001</v>
       </c>
       <c r="I80" s="7">
-        <f>AB58</f>
+        <f t="shared" si="68"/>
         <v>0</v>
       </c>
       <c r="J80" s="10">
-        <f>IFERROR(L80/G80,S58)</f>
+        <f t="shared" si="69"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K80">
-        <f t="shared" si="31"/>
+        <f t="shared" si="71"/>
         <v>1.2</v>
       </c>
       <c r="L80">
-        <f>P58</f>
+        <f t="shared" si="70"/>
         <v>0</v>
       </c>
       <c r="M80" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="72"/>
         <v>0</v>
       </c>
       <c r="N80">
-        <f t="shared" si="33"/>
+        <f t="shared" si="73"/>
         <v>0.10001</v>
       </c>
     </row>
@@ -8081,39 +8083,39 @@
         <v>98</v>
       </c>
       <c r="F81" s="7">
-        <f>O59</f>
+        <f t="shared" si="66"/>
         <v>0.59816812053925483</v>
       </c>
       <c r="G81" s="7">
-        <f>T59</f>
+        <f t="shared" si="67"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="H81" s="7">
-        <f>AA59</f>
+        <f t="shared" si="68"/>
         <v>2</v>
       </c>
       <c r="I81" s="7">
-        <f>AB59</f>
-        <v>0.99694686756542472</v>
+        <f t="shared" si="68"/>
+        <v>0.24923671689135618</v>
       </c>
       <c r="J81" s="10">
-        <f>IFERROR(L81/G81,S59)</f>
+        <f t="shared" si="69"/>
         <v>0.66666666666666674</v>
       </c>
       <c r="K81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="71"/>
         <v>1.2</v>
       </c>
       <c r="L81">
-        <f>P59</f>
+        <f t="shared" si="70"/>
         <v>0.49847343378271236</v>
       </c>
       <c r="M81" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="72"/>
         <v>3.6643151526566218</v>
       </c>
       <c r="N81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="73"/>
         <v>0.10001</v>
       </c>
     </row>
@@ -8134,39 +8136,39 @@
         <v>7</v>
       </c>
       <c r="F82" s="7">
-        <f>O60</f>
+        <f t="shared" si="66"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="G82" s="7">
-        <f>T60</f>
+        <f t="shared" si="67"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="H82" s="7">
-        <f>AA60</f>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="I82" s="7">
-        <f>AB60</f>
+        <f t="shared" si="68"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="J82" s="10">
-        <f>IFERROR(L82/G82,S60)</f>
+        <f t="shared" si="69"/>
         <v>0.5</v>
       </c>
       <c r="K82">
-        <f t="shared" si="31"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="L82">
-        <f>P60</f>
+        <f t="shared" si="70"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="M82" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="72"/>
         <v>7.3286303053132436</v>
       </c>
       <c r="N82">
-        <f t="shared" si="33"/>
+        <f t="shared" si="73"/>
         <v>0.10001</v>
       </c>
     </row>
@@ -8187,39 +8189,39 @@
         <v>8</v>
       </c>
       <c r="F83" s="7">
-        <f>O61</f>
+        <f t="shared" si="66"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="G83" s="7">
-        <f>T61</f>
+        <f t="shared" si="67"/>
         <v>1.4954203013481369</v>
       </c>
       <c r="H83" s="7">
-        <f>AA61</f>
+        <f t="shared" si="68"/>
         <v>1</v>
       </c>
       <c r="I83" s="7">
-        <f>AB61</f>
+        <f t="shared" si="68"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="J83" s="10">
-        <f>IFERROR(L83/G83,S61)</f>
+        <f t="shared" si="69"/>
         <v>0.5</v>
       </c>
       <c r="K83">
-        <f t="shared" si="31"/>
+        <f t="shared" si="71"/>
         <v>1</v>
       </c>
       <c r="L83">
-        <f>P61</f>
+        <f t="shared" si="70"/>
         <v>0.74771015067406843</v>
       </c>
       <c r="M83" s="11">
-        <f t="shared" si="32"/>
+        <f t="shared" si="72"/>
         <v>7.3286303053132436</v>
       </c>
       <c r="N83">
-        <f t="shared" si="33"/>
+        <f t="shared" si="73"/>
         <v>0.10001</v>
       </c>
     </row>

</xml_diff>